<commit_message>
cost-down on LEDs, LDO, reverse polarity fet. also got rid of all old traces, starting new placement
</commit_message>
<xml_diff>
--- a/PHANTOM_VCU/Project Outputs for PHANTOM_VCU/TEST_BOM.xlsx
+++ b/PHANTOM_VCU/Project Outputs for PHANTOM_VCU/TEST_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel\Documents\Phantom\vcu-hw\PHANTOM_VCU\Project Outputs for PHANTOM_VCU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFE42BC-EFF7-4DCE-B753-0326E434492D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BD64DD-2887-440B-BCE7-3332FEA23DE6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7155" xr2:uid="{6F62929B-99FA-4639-A2B5-5ECB069F5532}"/>
   </bookViews>
@@ -24,6 +24,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>gabe</author>
+  </authors>
+  <commentList>
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{38E8DF1C-52B7-4AA7-B471-01D0CAFB5EBA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>gabe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+there is a cheaper one @ 0.21 each.. But no price break until 0.189 at 50 minimum..</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="302">
   <si>
@@ -937,7 +971,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -965,8 +999,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -981,18 +1028,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEEEEEE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1024,25 +1065,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1054,11 +1082,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1373,11 +1398,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EB8FEE-8E75-4FD7-9358-958697ECE29D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EB8FEE-8E75-4FD7-9358-958697ECE29D}">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,7 +1637,7 @@
       <c r="L6" s="5">
         <v>0.21199999999999999</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="8">
         <f t="shared" si="1"/>
         <v>5.3</v>
       </c>
@@ -1652,7 +1677,7 @@
       <c r="L7" s="5">
         <v>0.35099999999999998</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="8">
         <f t="shared" si="1"/>
         <v>8.7749999999999986</v>
       </c>
@@ -1760,24 +1785,24 @@
         <v>3</v>
       </c>
       <c r="H10">
-        <v>0.43</v>
+        <v>0.21</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
-        <v>1.29</v>
+        <f>H10*G10</f>
+        <v>0.63</v>
       </c>
       <c r="K10">
         <v>25</v>
       </c>
       <c r="L10" s="5">
-        <v>0.2288</v>
-      </c>
-      <c r="M10" s="9">
-        <f t="shared" si="1"/>
-        <v>5.72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.21</v>
+      </c>
+      <c r="M10" s="8">
+        <f t="shared" si="1"/>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -1800,21 +1825,21 @@
         <v>3</v>
       </c>
       <c r="H11">
-        <v>3.9266700000000001</v>
+        <v>0.21</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>11.780010000000001</v>
+        <v>0.63</v>
       </c>
       <c r="K11">
         <v>25</v>
       </c>
-      <c r="L11" s="7">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="M11" s="9">
-        <f t="shared" si="1"/>
-        <v>10.6</v>
+      <c r="L11">
+        <v>0.21</v>
+      </c>
+      <c r="M11" s="8">
+        <f t="shared" si="1"/>
+        <v>5.25</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1852,7 +1877,7 @@
       <c r="L12" s="5">
         <v>0.64900000000000002</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="8">
         <f t="shared" si="1"/>
         <v>12.98</v>
       </c>
@@ -1880,21 +1905,21 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0.43</v>
+        <v>0.21</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>0.43</v>
+        <v>0.21</v>
       </c>
       <c r="K13">
         <v>5</v>
       </c>
-      <c r="L13" s="8">
-        <v>0.43</v>
-      </c>
-      <c r="M13" s="9">
-        <f t="shared" si="1"/>
-        <v>2.15</v>
+      <c r="L13" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="M13" s="8">
+        <f t="shared" si="1"/>
+        <v>1.05</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1929,10 +1954,10 @@
       <c r="K14">
         <v>5</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="7">
         <v>0.74</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="8">
         <f t="shared" si="1"/>
         <v>3.7</v>
       </c>
@@ -1969,10 +1994,10 @@
       <c r="K15">
         <v>5</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="7">
         <v>0.75</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="8">
         <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
@@ -2237,7 +2262,7 @@
       <c r="L22" s="5">
         <v>0.75</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M22" s="8">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
@@ -2277,7 +2302,7 @@
       <c r="L23" s="5">
         <v>0.8</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M23" s="8">
         <f t="shared" si="1"/>
         <v>4.8000000000000007</v>
       </c>
@@ -2318,11 +2343,11 @@
         <v>5</v>
       </c>
       <c r="L24">
-        <v>5.58</v>
-      </c>
-      <c r="M24" s="9">
-        <f t="shared" si="1"/>
-        <v>27.9</v>
+        <v>1.46</v>
+      </c>
+      <c r="M24" s="8">
+        <f t="shared" si="1"/>
+        <v>7.3</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -2360,7 +2385,7 @@
       <c r="L25" s="5">
         <v>1.903</v>
       </c>
-      <c r="M25" s="9">
+      <c r="M25" s="8">
         <f t="shared" si="1"/>
         <v>19.03</v>
       </c>
@@ -2563,7 +2588,7 @@
       <c r="L30" s="5">
         <v>0.89</v>
       </c>
-      <c r="M30" s="9">
+      <c r="M30" s="8">
         <f t="shared" si="1"/>
         <v>5.34</v>
       </c>
@@ -2723,7 +2748,7 @@
       <c r="L34" s="5">
         <v>0.11600000000000001</v>
       </c>
-      <c r="M34" s="9">
+      <c r="M34" s="8">
         <f t="shared" si="1"/>
         <v>1.1600000000000001</v>
       </c>
@@ -2966,7 +2991,7 @@
       <c r="L40" s="5">
         <v>5.18</v>
       </c>
-      <c r="M40" s="9">
+      <c r="M40" s="8">
         <f t="shared" si="1"/>
         <v>25.9</v>
       </c>
@@ -3049,7 +3074,7 @@
       <c r="L42" s="5">
         <v>2.2269999999999999</v>
       </c>
-      <c r="M42" s="9">
+      <c r="M42" s="8">
         <f t="shared" si="1"/>
         <v>26.723999999999997</v>
       </c>
@@ -3243,7 +3268,7 @@
       <c r="L47" s="5">
         <v>7.05</v>
       </c>
-      <c r="M47" s="9">
+      <c r="M47" s="8">
         <f t="shared" si="1"/>
         <v>35.25</v>
       </c>
@@ -3347,7 +3372,7 @@
       <c r="L50" s="5">
         <v>1.1599999999999999</v>
       </c>
-      <c r="M50" s="9">
+      <c r="M50" s="8">
         <f t="shared" si="1"/>
         <v>5.8</v>
       </c>
@@ -3430,7 +3455,7 @@
       <c r="L52" s="5">
         <v>4.26</v>
       </c>
-      <c r="M52" s="9">
+      <c r="M52" s="8">
         <f t="shared" si="1"/>
         <v>21.299999999999997</v>
       </c>
@@ -3561,11 +3586,11 @@
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I57">
         <f>SUM(I2:I55)</f>
-        <v>100.48400999999998</v>
+        <v>88.454000000000008</v>
       </c>
       <c r="M57">
-        <f t="shared" ref="J57:M57" si="2">SUM(M2:M55)</f>
-        <v>336.84900000000005</v>
+        <f t="shared" ref="M57" si="2">SUM(M2:M55)</f>
+        <v>309.32900000000001</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -3631,5 +3656,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId54"/>
+  <legacyDrawing r:id="rId55"/>
 </worksheet>
 </file>
</xml_diff>